<commit_message>
added new ML features
</commit_message>
<xml_diff>
--- a/simulated_stock_data_sample.xlsx
+++ b/simulated_stock_data_sample.xlsx
@@ -408,10 +408,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3028.264182043828</v>
+        <v>723.4437431232132</v>
       </c>
       <c r="C2">
-        <v>0.7741824307430223</v>
+        <v>-0.8981173803817657</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -422,10 +422,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2946.595163512278</v>
+        <v>742.0828156631055</v>
       </c>
       <c r="C3">
-        <v>-2.696892134306142</v>
+        <v>2.576437037028583</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -436,10 +436,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2929.627599190526</v>
+        <v>722.5588047460285</v>
       </c>
       <c r="C4">
-        <v>-0.5758362917261686</v>
+        <v>-2.630974670883721</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -450,10 +450,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2915.902541757709</v>
+        <v>726.9225315734888</v>
       </c>
       <c r="C5">
-        <v>-0.468491539218484</v>
+        <v>0.603926877480098</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -464,13 +464,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2951.802415604216</v>
+        <v>690.1473964039744</v>
       </c>
       <c r="C6">
-        <v>1.231175367914266</v>
+        <v>-5.059017099100123</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -478,13 +478,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2909.661413743241</v>
+        <v>673.5119594815275</v>
       </c>
       <c r="C7">
-        <v>-1.42763626854573</v>
+        <v>-2.410417978699365</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -492,13 +492,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2865.647332191137</v>
+        <v>708.3011407080222</v>
       </c>
       <c r="C8">
-        <v>-1.512687398754083</v>
+        <v>5.165339788958696</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -506,13 +506,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2901.311728739387</v>
+        <v>716.9031470278009</v>
       </c>
       <c r="C9">
-        <v>1.244549395440782</v>
+        <v>1.2144560873049</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -520,13 +520,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2904.718847864596</v>
+        <v>737.0237678958969</v>
       </c>
       <c r="C10">
-        <v>0.1174337487233576</v>
+        <v>2.806602391343067</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -534,13 +534,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2903.718191084606</v>
+        <v>754.4418310307557</v>
       </c>
       <c r="C11">
-        <v>-0.03444935060500552</v>
+        <v>2.363297344478466</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -548,13 +548,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>2952.800676100124</v>
+        <v>737.1391537247673</v>
       </c>
       <c r="C12">
-        <v>1.690332249397291</v>
+        <v>-2.29344087169035</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -562,13 +562,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>3051.363931150852</v>
+        <v>786.5039976230943</v>
       </c>
       <c r="C13">
-        <v>3.337958293239892</v>
+        <v>6.696814793907795</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -576,13 +576,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>3059.491987895841</v>
+        <v>813.616743146771</v>
       </c>
       <c r="C14">
-        <v>0.2663745435938024</v>
+        <v>3.447248279171446</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -590,13 +590,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>3080.333377479741</v>
+        <v>796.3368256892269</v>
       </c>
       <c r="C15">
-        <v>0.6812042543779755</v>
+        <v>-2.123839953282147</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -604,13 +604,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>3054.040087570233</v>
+        <v>773.2071555979192</v>
       </c>
       <c r="C16">
-        <v>-0.8535858521593067</v>
+        <v>-2.904508412164542</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -618,13 +618,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>2944.76362247064</v>
+        <v>770.4259874286001</v>
       </c>
       <c r="C17">
-        <v>-3.57809530871389</v>
+        <v>-0.3596925027379414</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -632,13 +632,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>3017.129985030717</v>
+        <v>754.1042732132172</v>
       </c>
       <c r="C18">
-        <v>2.457459132131023</v>
+        <v>-2.118531108985415</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -646,13 +646,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>3046.848817364699</v>
+        <v>774.3037031265424</v>
       </c>
       <c r="C19">
-        <v>0.9850033800807414</v>
+        <v>2.678599051992627</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -660,13 +660,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>3114.114027402327</v>
+        <v>792.2727885802718</v>
       </c>
       <c r="C20">
-        <v>2.20769765976795</v>
+        <v>2.320676677790964</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -674,13 +674,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>3149.643245460357</v>
+        <v>770.2773189884023</v>
       </c>
       <c r="C21">
-        <v>1.140909348385909</v>
+        <v>-2.776249532851522</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -688,13 +688,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>3161.411155490855</v>
+        <v>779.0778176555366</v>
       </c>
       <c r="C22">
-        <v>0.3736267606643613</v>
+        <v>1.142510424517222</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -702,13 +702,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>3143.081786106165</v>
+        <v>774.2547573828158</v>
       </c>
       <c r="C23">
-        <v>-0.5797844216768331</v>
+        <v>-0.6190729813402691</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -716,13 +716,13 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>3178.581780374465</v>
+        <v>783.8371951193577</v>
       </c>
       <c r="C24">
-        <v>1.129464540987307</v>
+        <v>1.237633691646021</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -730,13 +730,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>3236.001443878935</v>
+        <v>786.2861785271881</v>
       </c>
       <c r="C25">
-        <v>1.806455440567767</v>
+        <v>0.3124352127047796</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -744,13 +744,13 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>3358.360454824651</v>
+        <v>780.5623047291261</v>
       </c>
       <c r="C26">
-        <v>3.781179120830239</v>
+        <v>-0.727963170964478</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -758,13 +758,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3420.103068409203</v>
+        <v>801.4898390180426</v>
       </c>
       <c r="C27">
-        <v>1.838474887228148</v>
+        <v>2.681084413393351</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -772,13 +772,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>3431.554944574349</v>
+        <v>772.9530938267631</v>
       </c>
       <c r="C28">
-        <v>0.3348400892044635</v>
+        <v>-3.560462503959097</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -786,13 +786,13 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>3442.922146198314</v>
+        <v>753.897181304619</v>
       </c>
       <c r="C29">
-        <v>0.3312551250836754</v>
+        <v>-2.465338799253832</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -800,13 +800,13 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>3496.574310185435</v>
+        <v>786.2546487908779</v>
       </c>
       <c r="C30">
-        <v>1.558332187277723</v>
+        <v>4.292026590451532</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -814,13 +814,13 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>3506.580248002977</v>
+        <v>827.2184414684899</v>
       </c>
       <c r="C31">
-        <v>0.286164025983787</v>
+        <v>5.209990521595915</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -828,13 +828,13 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>3484.774914208669</v>
+        <v>861.5964676389304</v>
       </c>
       <c r="C32">
-        <v>-0.6218404329039864</v>
+        <v>4.155858289306527</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -842,13 +842,13 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>3525.53740746807</v>
+        <v>874.8669820655902</v>
       </c>
       <c r="C33">
-        <v>1.169731023177349</v>
+        <v>1.540223866402971</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -856,13 +856,13 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>3568.714700788704</v>
+        <v>906.160323343961</v>
       </c>
       <c r="C34">
-        <v>1.224701040731328</v>
+        <v>3.576925626394785</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -870,13 +870,13 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>3607.44086772495</v>
+        <v>894.4042457863867</v>
       </c>
       <c r="C35">
-        <v>1.085157267620399</v>
+        <v>-1.297350728642739</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -884,13 +884,13 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>3517.738898559504</v>
+        <v>888.9586072681379</v>
       </c>
       <c r="C36">
-        <v>-2.486581830571108</v>
+        <v>-0.6088565147027919</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -898,13 +898,13 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>3512.803366869138</v>
+        <v>889.0828903730277</v>
       </c>
       <c r="C37">
-        <v>-0.1403040939845552</v>
+        <v>0.01398075274524485</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -912,13 +912,13 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>3519.02289258246</v>
+        <v>905.3812987544659</v>
       </c>
       <c r="C38">
-        <v>0.1770530560287282</v>
+        <v>1.833170850312956</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -926,13 +926,13 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>3455.281502316276</v>
+        <v>871.2784941318116</v>
       </c>
       <c r="C39">
-        <v>-1.811337755163256</v>
+        <v>-3.766678709795479</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -940,13 +940,13 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>3434.063605902171</v>
+        <v>843.2096372008062</v>
       </c>
       <c r="C40">
-        <v>-0.6140714265937908</v>
+        <v>-3.221571187634408</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -954,13 +954,13 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>3388.538204017496</v>
+        <v>828.0880985548833</v>
       </c>
       <c r="C41">
-        <v>-1.325700601655401</v>
+        <v>-1.793330860890267</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -968,13 +968,13 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>3413.475342924697</v>
+        <v>820.1687880262729</v>
       </c>
       <c r="C42">
-        <v>0.7359261547541252</v>
+        <v>-0.9563367161574562</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -982,13 +982,13 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>3478.52516459718</v>
+        <v>852.0324074178183</v>
       </c>
       <c r="C43">
-        <v>1.905677209806594</v>
+        <v>3.885007556581719</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -996,13 +996,13 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>3523.649397790206</v>
+        <v>844.4563867844745</v>
       </c>
       <c r="C44">
-        <v>1.297223135030877</v>
+        <v>-0.8891704784215647</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1010,13 +1010,13 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>3546.330754879799</v>
+        <v>856.962626213446</v>
       </c>
       <c r="C45">
-        <v>0.6436893836207933</v>
+        <v>1.480981093244244</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1024,13 +1024,13 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>3555.506175841149</v>
+        <v>900.0302121095216</v>
       </c>
       <c r="C46">
-        <v>0.2587299830599476</v>
+        <v>5.025608419631193</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1038,13 +1038,13 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>3554.491798927641</v>
+        <v>837.9046008010069</v>
       </c>
       <c r="C47">
-        <v>-0.02852974691483835</v>
+        <v>-6.902613987024116</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1052,13 +1052,13 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>3444.478257310193</v>
+        <v>851.640952775248</v>
       </c>
       <c r="C48">
-        <v>-3.095056841898952</v>
+        <v>1.639369441474554</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1066,13 +1066,13 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>3394.034371869649</v>
+        <v>890.6855176685812</v>
       </c>
       <c r="C49">
-        <v>-1.464485523561882</v>
+        <v>4.584627449642752</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1080,13 +1080,13 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>3355.632864562541</v>
+        <v>861.2260203871737</v>
       </c>
       <c r="C50">
-        <v>-1.131441320258468</v>
+        <v>-3.307508284014693</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1094,13 +1094,13 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>3397.957336082679</v>
+        <v>841.4906629709401</v>
       </c>
       <c r="C51">
-        <v>1.261296251062194</v>
+        <v>-2.291542167683382</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1108,13 +1108,13 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>3383.150728610776</v>
+        <v>803.2224678420635</v>
       </c>
       <c r="C52">
-        <v>-0.4357502466164666</v>
+        <v>-4.547667230646173</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1122,13 +1122,13 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>3437.779890873763</v>
+        <v>778.2544431192504</v>
       </c>
       <c r="C53">
-        <v>1.614742192861712</v>
+        <v>-3.108481861804999</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1136,13 +1136,13 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>3607.215626938402</v>
+        <v>741.6398441975543</v>
       </c>
       <c r="C54">
-        <v>4.928638291079618</v>
+        <v>-4.704707984055236</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1150,13 +1150,13 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>3599.974567607846</v>
+        <v>765.357795807389</v>
       </c>
       <c r="C55">
-        <v>-0.2007381892138735</v>
+        <v>3.198041717337505</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1164,13 +1164,13 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>3608.693037065293</v>
+        <v>753.64294551583</v>
       </c>
       <c r="C56">
-        <v>0.242181418054845</v>
+        <v>-1.530637089702714</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1178,13 +1178,13 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>3502.837455084568</v>
+        <v>742.0319054032028</v>
       </c>
       <c r="C57">
-        <v>-2.933349578184419</v>
+        <v>-1.540655317178086</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1192,13 +1192,13 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>3428.720709062012</v>
+        <v>734.6702359484225</v>
       </c>
       <c r="C58">
-        <v>-2.115905946905161</v>
+        <v>-0.9920960812028992</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1206,13 +1206,13 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>3385.039358389856</v>
+        <v>751.9340230423495</v>
       </c>
       <c r="C59">
-        <v>-1.273983925162159</v>
+        <v>2.349868859412862</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1220,13 +1220,13 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>3416.395750564308</v>
+        <v>762.3391708459318</v>
       </c>
       <c r="C60">
-        <v>0.926322823890809</v>
+        <v>1.383784678539045</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1234,13 +1234,13 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>3468.648830013998</v>
+        <v>763.1275117767337</v>
       </c>
       <c r="C61">
-        <v>1.529479699213947</v>
+        <v>0.1034107862943957</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1248,13 +1248,13 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>3461.068019832961</v>
+        <v>757.1366714521893</v>
       </c>
       <c r="C62">
-        <v>-0.2185522534146672</v>
+        <v>-0.7850379172671259</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1262,13 +1262,13 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>3448.492924577239</v>
+        <v>777.0654962340558</v>
       </c>
       <c r="C63">
-        <v>-0.3633299080995285</v>
+        <v>2.632130437381014</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1276,13 +1276,13 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>3394.56433113618</v>
+        <v>790.1229838010333</v>
       </c>
       <c r="C64">
-        <v>-1.563830769572213</v>
+        <v>1.680358686656257</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1290,13 +1290,13 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>3430.827142986328</v>
+        <v>784.5711850272011</v>
       </c>
       <c r="C65">
-        <v>1.068261146726054</v>
+        <v>-0.7026499529382547</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1304,13 +1304,13 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>3529.72738451617</v>
+        <v>780.3639229405646</v>
       </c>
       <c r="C66">
-        <v>2.882693805545536</v>
+        <v>-0.5362498861707012</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1318,13 +1318,13 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>3538.802124164892</v>
+        <v>746.042378395916</v>
       </c>
       <c r="C67">
-        <v>0.2570946325353503</v>
+        <v>-4.398145984929488</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1332,13 +1332,13 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>3506.385123502304</v>
+        <v>743.907866384085</v>
       </c>
       <c r="C68">
-        <v>-0.9160444558690071</v>
+        <v>-0.2861113622553828</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1346,13 +1346,13 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>3523.979395419786</v>
+        <v>726.6464064668573</v>
       </c>
       <c r="C69">
-        <v>0.5017780790692912</v>
+        <v>-2.320376043491848</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1360,13 +1360,13 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>3552.195770620935</v>
+        <v>736.3465187351139</v>
       </c>
       <c r="C70">
-        <v>0.8006963729079399</v>
+        <v>1.334915053859692</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1374,13 +1374,13 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>3607.4095980447</v>
+        <v>717.557594039803</v>
       </c>
       <c r="C71">
-        <v>1.554357670273156</v>
+        <v>-2.551641681906276</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1388,13 +1388,13 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>3621.886083882197</v>
+        <v>684.9322726904899</v>
       </c>
       <c r="C72">
-        <v>0.4012986450261694</v>
+        <v>-4.546718147826248</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1402,13 +1402,13 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>3603.796288431833</v>
+        <v>692.376657558674</v>
       </c>
       <c r="C73">
-        <v>-0.4994578799942411</v>
+        <v>1.086878975484943</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1416,13 +1416,13 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>3554.535228672295</v>
+        <v>667.3854702670039</v>
       </c>
       <c r="C74">
-        <v>-1.366921318989798</v>
+        <v>-3.60947860082245</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1430,13 +1430,13 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>3538.497709241997</v>
+        <v>698.4681914806821</v>
       </c>
       <c r="C75">
-        <v>-0.4511847090706377</v>
+        <v>4.65738656270756</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1444,13 +1444,13 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>3478.137022450271</v>
+        <v>719.4577929947658</v>
       </c>
       <c r="C76">
-        <v>-1.705828059011431</v>
+        <v>3.005090535273739</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1458,13 +1458,13 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>3532.759931523144</v>
+        <v>744.2255768554394</v>
       </c>
       <c r="C77">
-        <v>1.570464553877545</v>
+        <v>3.442562454925527</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1472,13 +1472,13 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>3418.000276632248</v>
+        <v>726.2004190068158</v>
       </c>
       <c r="C78">
-        <v>-3.248441929690291</v>
+        <v>-2.422001931831598</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1486,13 +1486,13 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>3319.547610470734</v>
+        <v>736.3366254606462</v>
       </c>
       <c r="C79">
-        <v>-2.880417150185817</v>
+        <v>1.395786368134181</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1500,13 +1500,13 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>3325.15258551845</v>
+        <v>740.2804404251606</v>
       </c>
       <c r="C80">
-        <v>0.1688475571200397</v>
+        <v>0.5355994565728819</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1514,13 +1514,13 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>3407.105378355305</v>
+        <v>736.1768819114421</v>
       </c>
       <c r="C81">
-        <v>2.464632546300935</v>
+        <v>-0.554324859827666</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1528,13 +1528,13 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>3451.711573712802</v>
+        <v>743.714959724336</v>
       </c>
       <c r="C82">
-        <v>1.309210910847409</v>
+        <v>1.023949270632037</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1542,13 +1542,13 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>3393.72313351118</v>
+        <v>742.2640253125825</v>
       </c>
       <c r="C83">
-        <v>-1.679990896204777</v>
+        <v>-0.1950928097898428</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1556,13 +1556,13 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>3307.043854393817</v>
+        <v>733.7846800176569</v>
       </c>
       <c r="C84">
-        <v>-2.554105791997356</v>
+        <v>-1.142362421694189</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1570,13 +1570,13 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>3262.223299273864</v>
+        <v>728.9613759228999</v>
       </c>
       <c r="C85">
-        <v>-1.355305738096062</v>
+        <v>-0.6573187238851748</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1584,13 +1584,13 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>3260.479663683133</v>
+        <v>761.2963995621634</v>
       </c>
       <c r="C86">
-        <v>-0.05344930223259352</v>
+        <v>4.435766380396461</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1598,13 +1598,13 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>3352.875574329232</v>
+        <v>762.2319582822192</v>
       </c>
       <c r="C87">
-        <v>2.833813431663181</v>
+        <v>0.1228902068358479</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1612,13 +1612,13 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>3344.966606994612</v>
+        <v>767.577432626388</v>
       </c>
       <c r="C88">
-        <v>-0.2358860971511838</v>
+        <v>0.7012923410106587</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1626,13 +1626,13 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>3356.003620414715</v>
+        <v>784.2220273967741</v>
       </c>
       <c r="C89">
-        <v>0.3299588521159978</v>
+        <v>2.16845806858</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1640,13 +1640,13 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>3374.830508882353</v>
+        <v>806.1042936565144</v>
       </c>
       <c r="C90">
-        <v>0.5609913038565719</v>
+        <v>2.790315178008773</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1654,13 +1654,13 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>3409.159098288151</v>
+        <v>817.4866373408665</v>
       </c>
       <c r="C91">
-        <v>1.017194472891242</v>
+        <v>1.412018739252887</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1668,13 +1668,13 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>3344.729291650104</v>
+        <v>815.9780487916818</v>
       </c>
       <c r="C92">
-        <v>-1.889903192561455</v>
+        <v>-0.1845398420323951</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1682,13 +1682,13 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>3333.666639976644</v>
+        <v>794.0485519524923</v>
       </c>
       <c r="C93">
-        <v>-0.3307487903752663</v>
+        <v>-2.687510634834249</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1696,13 +1696,13 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>3344.103179396201</v>
+        <v>807.3298739072225</v>
       </c>
       <c r="C94">
-        <v>0.3130648786055579</v>
+        <v>1.672608296063581</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1710,13 +1710,13 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>3346.069693869444</v>
+        <v>819.8036841537606</v>
       </c>
       <c r="C95">
-        <v>0.05880543654750234</v>
+        <v>1.545069822099955</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1724,13 +1724,13 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>3346.87752441118</v>
+        <v>818.1447356999787</v>
       </c>
       <c r="C96">
-        <v>0.02414266932980168</v>
+        <v>-0.2023592337834377</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1738,13 +1738,13 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>3277.760428183955</v>
+        <v>799.3139714290819</v>
       </c>
       <c r="C97">
-        <v>-2.065121765678717</v>
+        <v>-2.301642172736809</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1752,13 +1752,13 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>3299.912226222745</v>
+        <v>812.9659568311168</v>
       </c>
       <c r="C98">
-        <v>0.6758211444715998</v>
+        <v>1.707962814365262</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1766,13 +1766,13 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>3159.537430130074</v>
+        <v>829.8623449876394</v>
       </c>
       <c r="C99">
-        <v>-4.2538948453593</v>
+        <v>2.078363554408038</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1780,13 +1780,13 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>3174.578429207226</v>
+        <v>803.4165138157098</v>
       </c>
       <c r="C100">
-        <v>0.4760506691174911</v>
+        <v>-3.186773243979823</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1794,13 +1794,13 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>3142.877839671886</v>
+        <v>785.320480002772</v>
       </c>
       <c r="C101">
-        <v>-0.9985763540659123</v>
+        <v>-2.252385095620368</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1808,13 +1808,13 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>3115.405876848927</v>
+        <v>764.5612047683978</v>
       </c>
       <c r="C102">
-        <v>-0.8741021517345149</v>
+        <v>-2.643414473833774</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1822,13 +1822,13 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>3052.277450920973</v>
+        <v>754.5088703796673</v>
       </c>
       <c r="C103">
-        <v>-2.026330706925576</v>
+        <v>-1.314784784532133</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1836,13 +1836,13 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>3035.683997385316</v>
+        <v>747.691353392087</v>
       </c>
       <c r="C104">
-        <v>-0.543641716799049</v>
+        <v>-0.9035701573859205</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1850,13 +1850,13 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>3056.80146024562</v>
+        <v>765.540881038714</v>
       </c>
       <c r="C105">
-        <v>0.6956410113336127</v>
+        <v>2.387285551136609</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1864,13 +1864,13 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>3024.468474844658</v>
+        <v>780.759715318924</v>
       </c>
       <c r="C106">
-        <v>-1.057739137508915</v>
+        <v>1.987984529259957</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1878,13 +1878,13 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>3031.344131573377</v>
+        <v>769.2292921815265</v>
       </c>
       <c r="C107">
-        <v>0.2273343824181248</v>
+        <v>-1.476820961835557</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1892,13 +1892,13 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>3035.127399349625</v>
+        <v>767.9349256236519</v>
       </c>
       <c r="C108">
-        <v>0.1248049581980149</v>
+        <v>-0.1682679756258011</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1906,13 +1906,13 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>3017.181167685574</v>
+        <v>800.9368908986869</v>
       </c>
       <c r="C109">
-        <v>-0.5912842956080389</v>
+        <v>4.297495031656965</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1920,13 +1920,13 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>3018.822487832475</v>
+        <v>799.9846649514761</v>
       </c>
       <c r="C110">
-        <v>0.05439912473533084</v>
+        <v>-0.1188890108610532</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1934,13 +1934,13 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>3027.600474169612</v>
+        <v>830.4152894272262</v>
       </c>
       <c r="C111">
-        <v>0.2907751738473516</v>
+        <v>3.803900975726311</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1948,13 +1948,13 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>3072.336161200479</v>
+        <v>861.4157642032022</v>
       </c>
       <c r="C112">
-        <v>1.477595455957116</v>
+        <v>3.733129094643526</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -1962,13 +1962,13 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>3103.817690592787</v>
+        <v>872.6991230834269</v>
       </c>
       <c r="C113">
-        <v>1.024677240397004</v>
+        <v>1.30986213035719</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -1976,13 +1976,13 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>3223.695652906468</v>
+        <v>855.4019292441831</v>
       </c>
       <c r="C114">
-        <v>3.862274600631773</v>
+        <v>-1.982034057525947</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -1990,13 +1990,13 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>3294.667765258811</v>
+        <v>865.6642169436276</v>
       </c>
       <c r="C115">
-        <v>2.20157607894387</v>
+        <v>1.199703595304273</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2004,13 +2004,13 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>3317.37181521542</v>
+        <v>857.4117970441132</v>
       </c>
       <c r="C116">
-        <v>0.689115005646892</v>
+        <v>-0.9533049579721556</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2018,13 +2018,13 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>3355.355039679721</v>
+        <v>875.8473179634318</v>
       </c>
       <c r="C117">
-        <v>1.144979416840989</v>
+        <v>2.1501361402857</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2032,13 +2032,13 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>3322.598986099555</v>
+        <v>896.4200923118069</v>
       </c>
       <c r="C118">
-        <v>-0.9762321182944917</v>
+        <v>2.348899622848879</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2046,13 +2046,13 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>3332.961230570851</v>
+        <v>916.809803420873</v>
       </c>
       <c r="C119">
-        <v>0.3118716557323866</v>
+        <v>2.274570961086161</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2060,13 +2060,13 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>3314.16204624947</v>
+        <v>898.5918942666203</v>
       </c>
       <c r="C120">
-        <v>-0.5640384937259242</v>
+        <v>-1.987097987638934</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2074,13 +2074,13 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>3314.151903804779</v>
+        <v>882.1400580676907</v>
       </c>
       <c r="C121">
-        <v>-0.0003060334572993761</v>
+        <v>-1.830846272250958</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2088,13 +2088,13 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>3285.649831005326</v>
+        <v>844.9844610084057</v>
       </c>
       <c r="C122">
-        <v>-0.8600110564253682</v>
+        <v>-4.211983881638198</v>
       </c>
       <c r="D122">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2102,13 +2102,13 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>3341.07139040094</v>
+        <v>806.8004315071597</v>
       </c>
       <c r="C123">
-        <v>1.686776200939714</v>
+        <v>-4.518903158961897</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2116,13 +2116,13 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>3378.395011334439</v>
+        <v>852.5163560037225</v>
       </c>
       <c r="C124">
-        <v>1.117115337335562</v>
+        <v>5.666323753838634</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2130,13 +2130,13 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>3408.969337471928</v>
+        <v>820.1474633193247</v>
       </c>
       <c r="C125">
-        <v>0.9049955980550686</v>
+        <v>-3.796864711913693</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2144,13 +2144,13 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>3395.76656581275</v>
+        <v>800.5058271251943</v>
       </c>
       <c r="C126">
-        <v>-0.3872951133367882</v>
+        <v>-2.394890805933393</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2158,13 +2158,13 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>3459.633092490493</v>
+        <v>754.8208332765453</v>
       </c>
       <c r="C127">
-        <v>1.880769052876786</v>
+        <v>-5.707015776851327</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2172,13 +2172,13 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>3437.144925154236</v>
+        <v>734.7723026717637</v>
       </c>
       <c r="C128">
-        <v>-0.6500159622437869</v>
+        <v>-2.656064819747278</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2186,13 +2186,13 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>3419.263488454862</v>
+        <v>716.6441800273119</v>
       </c>
       <c r="C129">
-        <v>-0.5202409874693077</v>
+        <v>-2.467175556091964</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2200,13 +2200,13 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>3419.930591021335</v>
+        <v>738.4315650229362</v>
       </c>
       <c r="C130">
-        <v>0.01951012458456579</v>
+        <v>3.040195623272059</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2214,13 +2214,13 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>3378.828677205682</v>
+        <v>728.0896539528691</v>
       </c>
       <c r="C131">
-        <v>-1.201834736750554</v>
+        <v>-1.40052396998304</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2228,13 +2228,13 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>3381.982402881322</v>
+        <v>709.480982250343</v>
       </c>
       <c r="C132">
-        <v>0.09333783914277133</v>
+        <v>-2.555821470817194</v>
       </c>
       <c r="D132">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2242,13 +2242,13 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>3486.128374868257</v>
+        <v>684.7785921903227</v>
       </c>
       <c r="C133">
-        <v>3.079435655791908</v>
+        <v>-3.481755068567016</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2256,13 +2256,13 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>3486.183282772715</v>
+        <v>682.6574614715865</v>
       </c>
       <c r="C134">
-        <v>0.001575039658717969</v>
+        <v>-0.3097542392427166</v>
       </c>
       <c r="D134">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2270,13 +2270,13 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>3503.588446704348</v>
+        <v>663.8797000785727</v>
       </c>
       <c r="C135">
-        <v>0.4992612986713063</v>
+        <v>-2.750685732275626</v>
       </c>
       <c r="D135">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2284,13 +2284,13 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>3586.873204596248</v>
+        <v>664.1140574925739</v>
       </c>
       <c r="C136">
-        <v>2.377127312719661</v>
+        <v>0.03530118694298222</v>
       </c>
       <c r="D136">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2298,13 +2298,13 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>3672.850317171747</v>
+        <v>668.569622300642</v>
       </c>
       <c r="C137">
-        <v>2.396993360828231</v>
+        <v>0.6709035530569049</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2312,13 +2312,13 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>3693.249877077048</v>
+        <v>701.2923462562517</v>
       </c>
       <c r="C138">
-        <v>0.5554149541550173</v>
+        <v>4.894437746514139</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2326,13 +2326,13 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>3694.13055405652</v>
+        <v>678.1639931330021</v>
       </c>
       <c r="C139">
-        <v>0.02384558339629364</v>
+        <v>-3.297961719775913</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2340,13 +2340,13 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>3594.585068688776</v>
+        <v>673.8465616091755</v>
       </c>
       <c r="C140">
-        <v>-2.694693214305429</v>
+        <v>-0.6366353223621851</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2354,13 +2354,13 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>3592.932804688371</v>
+        <v>653.7789428606291</v>
       </c>
       <c r="C141">
-        <v>-0.04596536092015872</v>
+        <v>-2.978069473356678</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2368,13 +2368,13 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>3543.633814933582</v>
+        <v>702.6143884539896</v>
       </c>
       <c r="C142">
-        <v>-1.372109984647063</v>
+        <v>7.469718339302821</v>
       </c>
       <c r="D142">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2382,13 +2382,13 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>3569.054089628364</v>
+        <v>709.9013852728795</v>
       </c>
       <c r="C143">
-        <v>0.7173504945024669</v>
+        <v>1.037126045044988</v>
       </c>
       <c r="D143">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2396,13 +2396,13 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>3583.135606731113</v>
+        <v>703.63063646365</v>
       </c>
       <c r="C144">
-        <v>0.3945447939180736</v>
+        <v>-0.8833267464070323</v>
       </c>
       <c r="D144">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2410,13 +2410,13 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>3558.651904528812</v>
+        <v>680.3020859380686</v>
       </c>
       <c r="C145">
-        <v>-0.6833038123454405</v>
+        <v>-3.31545406306177</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2424,13 +2424,13 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>3617.082778510201</v>
+        <v>642.9451304431668</v>
       </c>
       <c r="C146">
-        <v>1.641938451665592</v>
+        <v>-5.491230479381858</v>
       </c>
       <c r="D146">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2438,13 +2438,13 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>3565.923232346203</v>
+        <v>642.1241597124711</v>
       </c>
       <c r="C147">
-        <v>-1.414386932694668</v>
+        <v>-0.127689081357508</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2452,13 +2452,13 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>3600.175482502051</v>
+        <v>645.0157744414919</v>
       </c>
       <c r="C148">
-        <v>0.9605436775853315</v>
+        <v>0.4503201889048481</v>
       </c>
       <c r="D148">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2466,13 +2466,13 @@
         <v>147</v>
       </c>
       <c r="B149">
-        <v>3718.017055216185</v>
+        <v>637.8722232892069</v>
       </c>
       <c r="C149">
-        <v>3.273217466395186</v>
+        <v>-1.107500224854259</v>
       </c>
       <c r="D149">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2480,13 +2480,13 @@
         <v>148</v>
       </c>
       <c r="B150">
-        <v>3883.703231863699</v>
+        <v>676.491126076557</v>
       </c>
       <c r="C150">
-        <v>4.456304911648114</v>
+        <v>6.054332102471956</v>
       </c>
       <c r="D150">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2494,13 +2494,13 @@
         <v>149</v>
       </c>
       <c r="B151">
-        <v>3821.855676276211</v>
+        <v>655.0028613648411</v>
       </c>
       <c r="C151">
-        <v>-1.592489227293729</v>
+        <v>-3.176429650502777</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2508,13 +2508,13 @@
         <v>150</v>
       </c>
       <c r="B152">
-        <v>3783.388908852125</v>
+        <v>678.3890991046145</v>
       </c>
       <c r="C152">
-        <v>-1.006494506395544</v>
+        <v>3.570402378249625</v>
       </c>
       <c r="D152">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2522,13 +2522,13 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>3680.162744557282</v>
+        <v>674.8232203465159</v>
       </c>
       <c r="C153">
-        <v>-2.728404792151312</v>
+        <v>-0.5256391594153091</v>
       </c>
       <c r="D153">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2536,13 +2536,13 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>3661.292719335272</v>
+        <v>659.118162662406</v>
       </c>
       <c r="C154">
-        <v>-0.5127497486331929</v>
+        <v>-2.327284718514207</v>
       </c>
       <c r="D154">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2550,13 +2550,13 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>3606.82031514038</v>
+        <v>660.5029979370336</v>
       </c>
       <c r="C155">
-        <v>-1.48779156354321</v>
+        <v>0.2101042503568297</v>
       </c>
       <c r="D155">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2564,13 +2564,13 @@
         <v>154</v>
       </c>
       <c r="B156">
-        <v>3720.143811789016</v>
+        <v>634.8806362057071</v>
       </c>
       <c r="C156">
-        <v>3.14192243436516</v>
+        <v>-3.87921959648229</v>
       </c>
       <c r="D156">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2578,13 +2578,13 @@
         <v>155</v>
       </c>
       <c r="B157">
-        <v>3712.349754468562</v>
+        <v>611.7800213988859</v>
       </c>
       <c r="C157">
-        <v>-0.2095095704567722</v>
+        <v>-3.638576055001377</v>
       </c>
       <c r="D157">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2592,13 +2592,13 @@
         <v>156</v>
       </c>
       <c r="B158">
-        <v>3786.497810606173</v>
+        <v>621.2751695659441</v>
       </c>
       <c r="C158">
-        <v>1.99733486987205</v>
+        <v>1.552052671701625</v>
       </c>
       <c r="D158">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2606,13 +2606,13 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>3843.397497751101</v>
+        <v>646.1505784510819</v>
       </c>
       <c r="C159">
-        <v>1.502699591837854</v>
+        <v>4.003927744692754</v>
       </c>
       <c r="D159">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2620,13 +2620,13 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>3872.756484466433</v>
+        <v>644.2523318436048</v>
       </c>
       <c r="C160">
-        <v>0.7638810904287441</v>
+        <v>-0.2937777463617642</v>
       </c>
       <c r="D160">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2634,13 +2634,13 @@
         <v>159</v>
       </c>
       <c r="B161">
-        <v>3967.447538843332</v>
+        <v>652.35411224825</v>
       </c>
       <c r="C161">
-        <v>2.445055731149221</v>
+        <v>1.257547703624289</v>
       </c>
       <c r="D161">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -2648,13 +2648,13 @@
         <v>160</v>
       </c>
       <c r="B162">
-        <v>3919.853485958814</v>
+        <v>635.3555006831645</v>
       </c>
       <c r="C162">
-        <v>-1.199613918484086</v>
+        <v>-2.60573379487133</v>
       </c>
       <c r="D162">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -2662,13 +2662,13 @@
         <v>161</v>
       </c>
       <c r="B163">
-        <v>3882.334417551613</v>
+        <v>652.6164236809562</v>
       </c>
       <c r="C163">
-        <v>-0.9571548666703058</v>
+        <v>2.71673464371239</v>
       </c>
       <c r="D163">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2676,13 +2676,13 @@
         <v>162</v>
       </c>
       <c r="B164">
-        <v>3923.923025508204</v>
+        <v>648.2278537143595</v>
       </c>
       <c r="C164">
-        <v>1.071226831170781</v>
+        <v>-0.6724577879673718</v>
       </c>
       <c r="D164">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -2690,13 +2690,13 @@
         <v>163</v>
       </c>
       <c r="B165">
-        <v>3895.788043403953</v>
+        <v>648.9114740263046</v>
       </c>
       <c r="C165">
-        <v>-0.7170115703430977</v>
+        <v>0.1054598792736063</v>
       </c>
       <c r="D165">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -2704,13 +2704,13 @@
         <v>164</v>
       </c>
       <c r="B166">
-        <v>3939.747338513971</v>
+        <v>656.2184744789657</v>
       </c>
       <c r="C166">
-        <v>1.128380050974458</v>
+        <v>1.126039644101729</v>
       </c>
       <c r="D166">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2718,13 +2718,13 @@
         <v>165</v>
       </c>
       <c r="B167">
-        <v>3904.936515047772</v>
+        <v>655.4777944080364</v>
       </c>
       <c r="C167">
-        <v>-0.8835800998174999</v>
+        <v>-0.1128709568131917</v>
       </c>
       <c r="D167">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -2732,13 +2732,13 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>3919.144399966106</v>
+        <v>670.8548291193412</v>
       </c>
       <c r="C168">
-        <v>0.3638441973021224</v>
+        <v>2.345927633626668</v>
       </c>
       <c r="D168">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2746,13 +2746,13 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>3947.252062019961</v>
+        <v>659.5790718806367</v>
       </c>
       <c r="C169">
-        <v>0.7171887326758957</v>
+        <v>-1.680804363219192</v>
       </c>
       <c r="D169">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2760,13 +2760,13 @@
         <v>168</v>
       </c>
       <c r="B170">
-        <v>3940.28456522349</v>
+        <v>664.8792417321969</v>
       </c>
       <c r="C170">
-        <v>-0.1765151220899027</v>
+        <v>0.8035685299183246</v>
       </c>
       <c r="D170">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2774,13 +2774,13 @@
         <v>169</v>
       </c>
       <c r="B171">
-        <v>3955.676199620485</v>
+        <v>664.2186163296868</v>
       </c>
       <c r="C171">
-        <v>0.3906224066363123</v>
+        <v>-0.09936020874843016</v>
       </c>
       <c r="D171">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -2788,13 +2788,13 @@
         <v>170</v>
       </c>
       <c r="B172">
-        <v>4019.435623495507</v>
+        <v>660.7459862587582</v>
       </c>
       <c r="C172">
-        <v>1.611846386242095</v>
+        <v>-0.5228143243135109</v>
       </c>
       <c r="D172">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2802,13 +2802,13 @@
         <v>171</v>
       </c>
       <c r="B173">
-        <v>4066.587126247772</v>
+        <v>686.697080945069</v>
       </c>
       <c r="C173">
-        <v>1.173087646351212</v>
+        <v>3.927544809352495</v>
       </c>
       <c r="D173">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -2816,13 +2816,13 @@
         <v>172</v>
       </c>
       <c r="B174">
-        <v>4081.033292365387</v>
+        <v>667.3714966588177</v>
       </c>
       <c r="C174">
-        <v>0.3552405412482549</v>
+        <v>-2.814280826657143</v>
       </c>
       <c r="D174">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -2830,13 +2830,13 @@
         <v>173</v>
       </c>
       <c r="B175">
-        <v>4031.980667265317</v>
+        <v>720.7048760802354</v>
       </c>
       <c r="C175">
-        <v>-1.201965815663296</v>
+        <v>7.991557878697275</v>
       </c>
       <c r="D175">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -2844,13 +2844,13 @@
         <v>174</v>
       </c>
       <c r="B176">
-        <v>4051.395083997298</v>
+        <v>724.1504165408379</v>
       </c>
       <c r="C176">
-        <v>0.4815106602470187</v>
+        <v>0.478079249212534</v>
       </c>
       <c r="D176">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -2858,13 +2858,13 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>4046.717772858559</v>
+        <v>714.3135407655851</v>
       </c>
       <c r="C177">
-        <v>-0.1154493956221252</v>
+        <v>-1.358402280874479</v>
       </c>
       <c r="D177">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -2872,13 +2872,13 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>3912.912681192802</v>
+        <v>691.0567295941324</v>
       </c>
       <c r="C178">
-        <v>-3.306509106298223</v>
+        <v>-3.255826726527767</v>
       </c>
       <c r="D178">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -2886,13 +2886,13 @@
         <v>177</v>
       </c>
       <c r="B179">
-        <v>3958.198471852513</v>
+        <v>697.6754075445198</v>
       </c>
       <c r="C179">
-        <v>1.157342224307089</v>
+        <v>0.9577618836408156</v>
       </c>
       <c r="D179">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -2900,13 +2900,13 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>3985.202906748573</v>
+        <v>734.245462913841</v>
       </c>
       <c r="C180">
-        <v>0.6822405467561523</v>
+        <v>5.241700506261233</v>
       </c>
       <c r="D180">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -2914,13 +2914,13 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>4097.696083185532</v>
+        <v>705.6618277311239</v>
       </c>
       <c r="C181">
-        <v>2.822771614626271</v>
+        <v>-3.892926361340174</v>
       </c>
       <c r="D181">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -2928,13 +2928,13 @@
         <v>180</v>
       </c>
       <c r="B182">
-        <v>4153.328789105429</v>
+        <v>710.6416820654994</v>
       </c>
       <c r="C182">
-        <v>1.357658176461155</v>
+        <v>0.7056998322251489</v>
       </c>
       <c r="D182">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -2942,13 +2942,13 @@
         <v>181</v>
       </c>
       <c r="B183">
-        <v>4182.048345367934</v>
+        <v>702.507330548498</v>
       </c>
       <c r="C183">
-        <v>0.6914828495600562</v>
+        <v>-1.144648804353642</v>
       </c>
       <c r="D183">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -2956,13 +2956,13 @@
         <v>182</v>
       </c>
       <c r="B184">
-        <v>4111.963462942817</v>
+        <v>689.7583731562041</v>
       </c>
       <c r="C184">
-        <v>-1.675850603275372</v>
+        <v>-1.814779268187827</v>
       </c>
       <c r="D184">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -2970,13 +2970,13 @@
         <v>183</v>
       </c>
       <c r="B185">
-        <v>4047.378154748515</v>
+        <v>660.313008877928</v>
       </c>
       <c r="C185">
-        <v>-1.570668338285304</v>
+        <v>-4.268939011720817</v>
       </c>
       <c r="D185">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -2984,13 +2984,13 @@
         <v>184</v>
       </c>
       <c r="B186">
-        <v>4116.029682039197</v>
+        <v>643.5435352654908</v>
       </c>
       <c r="C186">
-        <v>1.696197505294588</v>
+        <v>-2.539624903185483</v>
       </c>
       <c r="D186">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -2998,13 +2998,13 @@
         <v>185</v>
       </c>
       <c r="B187">
-        <v>4190.477609804381</v>
+        <v>652.1253216176763</v>
       </c>
       <c r="C187">
-        <v>1.808731557258859</v>
+        <v>1.333520714903158</v>
       </c>
       <c r="D187">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3012,13 +3012,13 @@
         <v>186</v>
       </c>
       <c r="B188">
-        <v>4194.802116886888</v>
+        <v>674.661187977893</v>
       </c>
       <c r="C188">
-        <v>0.1031984295152692</v>
+        <v>3.455756986143966</v>
       </c>
       <c r="D188">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3026,13 +3026,13 @@
         <v>187</v>
       </c>
       <c r="B189">
-        <v>4154.55488045913</v>
+        <v>667.2523745358096</v>
       </c>
       <c r="C189">
-        <v>-0.9594549470101592</v>
+        <v>-1.098153202541443</v>
       </c>
       <c r="D189">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3040,13 +3040,13 @@
         <v>188</v>
       </c>
       <c r="B190">
-        <v>4068.420867691471</v>
+        <v>698.933746204152</v>
       </c>
       <c r="C190">
-        <v>-2.07324286827425</v>
+        <v>4.748034308665045</v>
       </c>
       <c r="D190">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3054,13 +3054,13 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>4043.079896190628</v>
+        <v>701.3346939208715</v>
       </c>
       <c r="C191">
-        <v>-0.6228699617112841</v>
+        <v>0.3435157809676264</v>
       </c>
       <c r="D191">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3068,13 +3068,13 @@
         <v>190</v>
       </c>
       <c r="B192">
-        <v>3940.008809709609</v>
+        <v>684.9899828982858</v>
       </c>
       <c r="C192">
-        <v>-2.549321040579291</v>
+        <v>-2.33051511129574</v>
       </c>
       <c r="D192">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -3082,13 +3082,13 @@
         <v>191</v>
       </c>
       <c r="B193">
-        <v>3882.834681353193</v>
+        <v>672.9156134520292</v>
       </c>
       <c r="C193">
-        <v>-1.451116764397028</v>
+        <v>-1.762707447949567</v>
       </c>
       <c r="D193">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3096,13 +3096,13 @@
         <v>192</v>
       </c>
       <c r="B194">
-        <v>3837.087613780274</v>
+        <v>679.0081805326026</v>
       </c>
       <c r="C194">
-        <v>-1.178187363799267</v>
+        <v>0.9053983826172155</v>
       </c>
       <c r="D194">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3110,13 +3110,13 @@
         <v>193</v>
       </c>
       <c r="B195">
-        <v>3865.983977496442</v>
+        <v>689.708263329264</v>
       </c>
       <c r="C195">
-        <v>0.7530806336657989</v>
+        <v>1.575840041907657</v>
       </c>
       <c r="D195">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3124,13 +3124,13 @@
         <v>194</v>
       </c>
       <c r="B196">
-        <v>3852.984176386372</v>
+        <v>684.8753014167811</v>
       </c>
       <c r="C196">
-        <v>-0.3362611222845303</v>
+        <v>-0.7007255341778735</v>
       </c>
       <c r="D196">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3138,13 +3138,13 @@
         <v>195</v>
       </c>
       <c r="B197">
-        <v>3832.406172250922</v>
+        <v>690.2317372856613</v>
       </c>
       <c r="C197">
-        <v>-0.5340796430352791</v>
+        <v>0.7821038162420948</v>
       </c>
       <c r="D197">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3152,13 +3152,13 @@
         <v>196</v>
       </c>
       <c r="B198">
-        <v>3885.458965552799</v>
+        <v>707.4998021517471</v>
       </c>
       <c r="C198">
-        <v>1.384320735260603</v>
+        <v>2.501777871587376</v>
       </c>
       <c r="D198">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3166,13 +3166,13 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>3973.143384331685</v>
+        <v>704.3600190706013</v>
       </c>
       <c r="C199">
-        <v>2.256732590828186</v>
+        <v>-0.4437857186103333</v>
       </c>
       <c r="D199">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3180,13 +3180,13 @@
         <v>198</v>
       </c>
       <c r="B200">
-        <v>3974.493605346683</v>
+        <v>718.6647227089582</v>
       </c>
       <c r="C200">
-        <v>0.03398369714828536</v>
+        <v>2.030879557478547</v>
       </c>
       <c r="D200">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3194,13 +3194,13 @@
         <v>199</v>
       </c>
       <c r="B201">
-        <v>4060.300247438754</v>
+        <v>735.9888881257639</v>
       </c>
       <c r="C201">
-        <v>2.158932699668695</v>
+        <v>2.410604676893488</v>
       </c>
       <c r="D201">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added realtime date capabilities
</commit_message>
<xml_diff>
--- a/simulated_stock_data_sample.xlsx
+++ b/simulated_stock_data_sample.xlsx
@@ -408,10 +408,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>723.4437431232132</v>
+        <v>131.4839684554283</v>
       </c>
       <c r="C2">
-        <v>-0.8981173803817657</v>
+        <v>7.421541516589557</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -422,10 +422,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>742.0828156631055</v>
+        <v>131.5042338927397</v>
       </c>
       <c r="C3">
-        <v>2.576437037028583</v>
+        <v>0.01541285797004446</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -436,10 +436,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>722.5588047460285</v>
+        <v>135.6327968259183</v>
       </c>
       <c r="C4">
-        <v>-2.630974670883721</v>
+        <v>3.139490502295179</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -450,10 +450,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>726.9225315734888</v>
+        <v>131.9155325162224</v>
       </c>
       <c r="C5">
-        <v>0.603926877480098</v>
+        <v>-2.740682487338899</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -464,13 +464,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>690.1473964039744</v>
+        <v>127.9506838660694</v>
       </c>
       <c r="C6">
-        <v>-5.059017099100123</v>
+        <v>-3.005596516593191</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -478,13 +478,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>673.5119594815275</v>
+        <v>134.6219602521652</v>
       </c>
       <c r="C7">
-        <v>-2.410417978699365</v>
+        <v>5.213943516768371</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -492,13 +492,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>708.3011407080222</v>
+        <v>138.1509109189472</v>
       </c>
       <c r="C8">
-        <v>5.165339788958696</v>
+        <v>2.621378161610331</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -506,13 +506,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>716.9031470278009</v>
+        <v>141.2595643676476</v>
       </c>
       <c r="C9">
-        <v>1.2144560873049</v>
+        <v>2.250186718294107</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -520,13 +520,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>737.0237678958969</v>
+        <v>141.8147935613961</v>
       </c>
       <c r="C10">
-        <v>2.806602391343067</v>
+        <v>0.3930560003026601</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -534,13 +534,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>754.4418310307557</v>
+        <v>141.6356228088663</v>
       </c>
       <c r="C11">
-        <v>2.363297344478466</v>
+        <v>-0.1263413696344439</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -548,13 +548,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>737.1391537247673</v>
+        <v>137.7506090657956</v>
       </c>
       <c r="C12">
-        <v>-2.29344087169035</v>
+        <v>-2.742963716347997</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -562,13 +562,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>786.5039976230943</v>
+        <v>133.1222136274213</v>
       </c>
       <c r="C13">
-        <v>6.696814793907795</v>
+        <v>-3.359981832213611</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -576,13 +576,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>813.616743146771</v>
+        <v>139.7298214184994</v>
       </c>
       <c r="C14">
-        <v>3.447248279171446</v>
+        <v>4.963565141405524</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -590,13 +590,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>796.3368256892269</v>
+        <v>142.3557920478868</v>
       </c>
       <c r="C15">
-        <v>-2.123839953282147</v>
+        <v>1.879320106995995</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -604,13 +604,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>773.2071555979192</v>
+        <v>147.628468098183</v>
       </c>
       <c r="C16">
-        <v>-2.904508412164542</v>
+        <v>3.70387180910949</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -618,13 +618,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>770.4259874286001</v>
+        <v>152.0733297213824</v>
       </c>
       <c r="C17">
-        <v>-0.3596925027379414</v>
+        <v>3.010843152719852</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -632,13 +632,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>754.1042732132172</v>
+        <v>150.9597403120397</v>
       </c>
       <c r="C18">
-        <v>-2.118531108985415</v>
+        <v>-0.7322713400061234</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -646,13 +646,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>774.3037031265424</v>
+        <v>150.1529276182199</v>
       </c>
       <c r="C19">
-        <v>2.678599051992627</v>
+        <v>-0.5344555390411148</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -660,13 +660,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>792.2727885802718</v>
+        <v>150.5268713649432</v>
       </c>
       <c r="C20">
-        <v>2.320676677790964</v>
+        <v>0.2490419285556715</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -674,13 +674,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>770.2773189884023</v>
+        <v>152.8132482371499</v>
       </c>
       <c r="C21">
-        <v>-2.776249532851522</v>
+        <v>1.518916092173042</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -688,13 +688,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>779.0778176555366</v>
+        <v>161.0368850988799</v>
       </c>
       <c r="C22">
-        <v>1.142510424517222</v>
+        <v>5.381494704548012</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -702,13 +702,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>774.2547573828158</v>
+        <v>154.7154151669611</v>
       </c>
       <c r="C23">
-        <v>-0.6190729813402691</v>
+        <v>-3.925479512372154</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -716,13 +716,13 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>783.8371951193577</v>
+        <v>148.045593263557</v>
       </c>
       <c r="C24">
-        <v>1.237633691646021</v>
+        <v>-4.311026083733412</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -730,13 +730,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>786.2861785271881</v>
+        <v>140.9384255578355</v>
       </c>
       <c r="C25">
-        <v>0.3124352127047796</v>
+        <v>-4.800661437499839</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -744,13 +744,13 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>780.5623047291261</v>
+        <v>141.2802946313527</v>
       </c>
       <c r="C26">
-        <v>-0.727963170964478</v>
+        <v>0.2425662640717248</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -758,13 +758,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>801.4898390180426</v>
+        <v>143.9476691730932</v>
       </c>
       <c r="C27">
-        <v>2.681084413393351</v>
+        <v>1.888001825520393</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -772,13 +772,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>772.9530938267631</v>
+        <v>148.9200267589635</v>
       </c>
       <c r="C28">
-        <v>-3.560462503959097</v>
+        <v>3.454281416596706</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -786,13 +786,13 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>753.897181304619</v>
+        <v>154.7016340005523</v>
       </c>
       <c r="C29">
-        <v>-2.465338799253832</v>
+        <v>3.882357106305597</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -800,13 +800,13 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>786.2546487908779</v>
+        <v>162.8706575686858</v>
       </c>
       <c r="C30">
-        <v>4.292026590451532</v>
+        <v>5.280502446473364</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -814,13 +814,13 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>827.2184414684899</v>
+        <v>166.531373272464</v>
       </c>
       <c r="C31">
-        <v>5.209990521595915</v>
+        <v>2.247621369266224</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -828,13 +828,13 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>861.5964676389304</v>
+        <v>163.7956588874105</v>
       </c>
       <c r="C32">
-        <v>4.155858289306527</v>
+        <v>-1.642762160243275</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -842,13 +842,13 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>874.8669820655902</v>
+        <v>159.9187240000562</v>
       </c>
       <c r="C33">
-        <v>1.540223866402971</v>
+        <v>-2.366933845309803</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -856,13 +856,13 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>906.160323343961</v>
+        <v>162.1146471398976</v>
       </c>
       <c r="C34">
-        <v>3.576925626394785</v>
+        <v>1.373149488011582</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -870,13 +870,13 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>894.4042457863867</v>
+        <v>165.8927685140201</v>
       </c>
       <c r="C35">
-        <v>-1.297350728642739</v>
+        <v>2.330524379368478</v>
       </c>
       <c r="D35">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -884,13 +884,13 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>888.9586072681379</v>
+        <v>163.9540907659041</v>
       </c>
       <c r="C36">
-        <v>-0.6088565147027919</v>
+        <v>-1.168633066698201</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -898,13 +898,13 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>889.0828903730277</v>
+        <v>160.9049237609437</v>
       </c>
       <c r="C37">
-        <v>0.01398075274524485</v>
+        <v>-1.859768786930784</v>
       </c>
       <c r="D37">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -912,13 +912,13 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>905.3812987544659</v>
+        <v>165.4596283276288</v>
       </c>
       <c r="C38">
-        <v>1.833170850312956</v>
+        <v>2.830680665466796</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -926,13 +926,13 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>871.2784941318116</v>
+        <v>172.4556169106598</v>
       </c>
       <c r="C39">
-        <v>-3.766678709795479</v>
+        <v>4.228214854428461</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -940,13 +940,13 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>843.2096372008062</v>
+        <v>167.8080584443561</v>
       </c>
       <c r="C40">
-        <v>-3.221571187634408</v>
+        <v>-2.694930179462532</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -954,13 +954,13 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>828.0880985548833</v>
+        <v>174.1552893095287</v>
       </c>
       <c r="C41">
-        <v>-1.793330860890267</v>
+        <v>3.782435077322123</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -968,13 +968,13 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>820.1687880262729</v>
+        <v>175.658536666017</v>
       </c>
       <c r="C42">
-        <v>-0.9563367161574562</v>
+        <v>0.8631649158909961</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -982,13 +982,13 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>852.0324074178183</v>
+        <v>184.3898737489615</v>
       </c>
       <c r="C43">
-        <v>3.885007556581719</v>
+        <v>4.970630661432404</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -996,13 +996,13 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>844.4563867844745</v>
+        <v>181.8790430814415</v>
       </c>
       <c r="C44">
-        <v>-0.8891704784215647</v>
+        <v>-1.361696614065882</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1010,13 +1010,13 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>856.962626213446</v>
+        <v>175.9224635712509</v>
       </c>
       <c r="C45">
-        <v>1.480981093244244</v>
+        <v>-3.275022459582304</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1024,13 +1024,13 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>900.0302121095216</v>
+        <v>180.8753418544573</v>
       </c>
       <c r="C46">
-        <v>5.025608419631193</v>
+        <v>2.815375696009589</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1038,13 +1038,13 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>837.9046008010069</v>
+        <v>170.126000840201</v>
       </c>
       <c r="C47">
-        <v>-6.902613987024116</v>
+        <v>-5.942955465375599</v>
       </c>
       <c r="D47">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1052,13 +1052,13 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>851.640952775248</v>
+        <v>166.9921877803193</v>
       </c>
       <c r="C48">
-        <v>1.639369441474554</v>
+        <v>-1.842054150691121</v>
       </c>
       <c r="D48">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1066,13 +1066,13 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>890.6855176685812</v>
+        <v>168.8664210788557</v>
       </c>
       <c r="C49">
-        <v>4.584627449642752</v>
+        <v>1.122347891508568</v>
       </c>
       <c r="D49">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1080,13 +1080,13 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>861.2260203871737</v>
+        <v>170.138114956949</v>
       </c>
       <c r="C50">
-        <v>-3.307508284014693</v>
+        <v>0.7530768224781981</v>
       </c>
       <c r="D50">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1094,13 +1094,13 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>841.4906629709401</v>
+        <v>172.4780590689802</v>
       </c>
       <c r="C51">
-        <v>-2.291542167683382</v>
+        <v>1.375320346427515</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1108,13 +1108,13 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>803.2224678420635</v>
+        <v>171.4751836780319</v>
       </c>
       <c r="C52">
-        <v>-4.547667230646173</v>
+        <v>-0.5814509951942248</v>
       </c>
       <c r="D52">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1122,13 +1122,13 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>778.2544431192504</v>
+        <v>164.1973968517106</v>
       </c>
       <c r="C53">
-        <v>-3.108481861804999</v>
+        <v>-4.24422162450418</v>
       </c>
       <c r="D53">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1136,13 +1136,13 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>741.6398441975543</v>
+        <v>160.2549318787388</v>
       </c>
       <c r="C54">
-        <v>-4.704707984055236</v>
+        <v>-2.401052055978862</v>
       </c>
       <c r="D54">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1150,13 +1150,13 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>765.357795807389</v>
+        <v>164.1082179071822</v>
       </c>
       <c r="C55">
-        <v>3.198041717337505</v>
+        <v>2.404472663193352</v>
       </c>
       <c r="D55">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1164,13 +1164,13 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>753.64294551583</v>
+        <v>167.623464621983</v>
       </c>
       <c r="C56">
-        <v>-1.530637089702714</v>
+        <v>2.142029667757976</v>
       </c>
       <c r="D56">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1178,10 +1178,10 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>742.0319054032028</v>
+        <v>156.5337419141284</v>
       </c>
       <c r="C57">
-        <v>-1.540655317178086</v>
+        <v>-6.615853414594199</v>
       </c>
       <c r="D57">
         <v>6</v>
@@ -1192,10 +1192,10 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>734.6702359484225</v>
+        <v>163.1235811936487</v>
       </c>
       <c r="C58">
-        <v>-0.9920960812028992</v>
+        <v>4.209852265037754</v>
       </c>
       <c r="D58">
         <v>6</v>
@@ -1206,13 +1206,13 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>751.9340230423495</v>
+        <v>151.757605078876</v>
       </c>
       <c r="C59">
-        <v>2.349868859412862</v>
+        <v>-6.967708795750267</v>
       </c>
       <c r="D59">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1220,13 +1220,13 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>762.3391708459318</v>
+        <v>151.1093360215798</v>
       </c>
       <c r="C60">
-        <v>1.383784678539045</v>
+        <v>-0.4271740167217593</v>
       </c>
       <c r="D60">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1234,13 +1234,13 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>763.1275117767337</v>
+        <v>148.9738721083319</v>
       </c>
       <c r="C61">
-        <v>0.1034107862943957</v>
+        <v>-1.413191249111848</v>
       </c>
       <c r="D61">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1248,13 +1248,13 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>757.1366714521893</v>
+        <v>153.0187719325871</v>
       </c>
       <c r="C62">
-        <v>-0.7850379172671259</v>
+        <v>2.715173987901579</v>
       </c>
       <c r="D62">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1262,13 +1262,13 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>777.0654962340558</v>
+        <v>162.071130851887</v>
       </c>
       <c r="C63">
-        <v>2.632130437381014</v>
+        <v>5.915848627570976</v>
       </c>
       <c r="D63">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1276,13 +1276,13 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>790.1229838010333</v>
+        <v>162.0713280860986</v>
       </c>
       <c r="C64">
-        <v>1.680358686656257</v>
+        <v>0.0001216960791306301</v>
       </c>
       <c r="D64">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1290,13 +1290,13 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>784.5711850272011</v>
+        <v>164.5860855542054</v>
       </c>
       <c r="C65">
-        <v>-0.7026499529382547</v>
+        <v>1.551636244241094</v>
       </c>
       <c r="D65">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1304,13 +1304,13 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>780.3639229405646</v>
+        <v>172.7832390398936</v>
       </c>
       <c r="C66">
-        <v>-0.5362498861707012</v>
+        <v>4.980465668216237</v>
       </c>
       <c r="D66">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1318,13 +1318,13 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>746.042378395916</v>
+        <v>163.6604331385038</v>
       </c>
       <c r="C67">
-        <v>-4.398145984929488</v>
+        <v>-5.279913695380742</v>
       </c>
       <c r="D67">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1332,13 +1332,13 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>743.907866384085</v>
+        <v>163.410872921919</v>
       </c>
       <c r="C68">
-        <v>-0.2861113622553828</v>
+        <v>-0.1524865917797134</v>
       </c>
       <c r="D68">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1346,13 +1346,13 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>726.6464064668573</v>
+        <v>166.1229416906157</v>
       </c>
       <c r="C69">
-        <v>-2.320376043491848</v>
+        <v>1.659662371421603</v>
       </c>
       <c r="D69">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1360,13 +1360,13 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>736.3465187351139</v>
+        <v>167.7748018164131</v>
       </c>
       <c r="C70">
-        <v>1.334915053859692</v>
+        <v>0.9943600257656618</v>
       </c>
       <c r="D70">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1374,13 +1374,13 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>717.557594039803</v>
+        <v>166.6768574929207</v>
       </c>
       <c r="C71">
-        <v>-2.551641681906276</v>
+        <v>-0.6544155091262638</v>
       </c>
       <c r="D71">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1388,13 +1388,13 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>684.9322726904899</v>
+        <v>162.5490986684486</v>
       </c>
       <c r="C72">
-        <v>-4.546718147826248</v>
+        <v>-2.476503868959375</v>
       </c>
       <c r="D72">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1402,13 +1402,13 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>692.376657558674</v>
+        <v>164.8817341059455</v>
       </c>
       <c r="C73">
-        <v>1.086878975484943</v>
+        <v>1.435034372140541</v>
       </c>
       <c r="D73">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1416,13 +1416,13 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>667.3854702670039</v>
+        <v>165.6151277886904</v>
       </c>
       <c r="C74">
-        <v>-3.60947860082245</v>
+        <v>0.4447998359076264</v>
       </c>
       <c r="D74">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1430,13 +1430,13 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>698.4681914806821</v>
+        <v>159.9005517958765</v>
       </c>
       <c r="C75">
-        <v>4.65738656270756</v>
+        <v>-3.450515704160249</v>
       </c>
       <c r="D75">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1444,13 +1444,13 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>719.4577929947658</v>
+        <v>166.2012338524156</v>
       </c>
       <c r="C76">
-        <v>3.005090535273739</v>
+        <v>3.94037543071292</v>
       </c>
       <c r="D76">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1458,13 +1458,13 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>744.2255768554394</v>
+        <v>168.6702060358938</v>
       </c>
       <c r="C77">
-        <v>3.442562454925527</v>
+        <v>1.485531801569296</v>
       </c>
       <c r="D77">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1472,13 +1472,13 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>726.2004190068158</v>
+        <v>171.1118378308859</v>
       </c>
       <c r="C78">
-        <v>-2.422001931831598</v>
+        <v>1.447577407045141</v>
       </c>
       <c r="D78">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1486,13 +1486,13 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>736.3366254606462</v>
+        <v>175.5718270188978</v>
       </c>
       <c r="C79">
-        <v>1.395786368134181</v>
+        <v>2.606476117929253</v>
       </c>
       <c r="D79">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1500,13 +1500,13 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>740.2804404251606</v>
+        <v>176.9644479636871</v>
       </c>
       <c r="C80">
-        <v>0.5355994565728819</v>
+        <v>0.7931915777349698</v>
       </c>
       <c r="D80">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1514,13 +1514,13 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>736.1768819114421</v>
+        <v>172.2249784263869</v>
       </c>
       <c r="C81">
-        <v>-0.554324859827666</v>
+        <v>-2.678204346600038</v>
       </c>
       <c r="D81">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1528,13 +1528,13 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>743.714959724336</v>
+        <v>170.8128644938521</v>
       </c>
       <c r="C82">
-        <v>1.023949270632037</v>
+        <v>-0.8199240002450385</v>
       </c>
       <c r="D82">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1542,13 +1542,13 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>742.2640253125825</v>
+        <v>184.0225910788005</v>
       </c>
       <c r="C83">
-        <v>-0.1950928097898428</v>
+        <v>7.733449482327431</v>
       </c>
       <c r="D83">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1556,13 +1556,13 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>733.7846800176569</v>
+        <v>184.552320192064</v>
       </c>
       <c r="C84">
-        <v>-1.142362421694189</v>
+        <v>0.2878609143355941</v>
       </c>
       <c r="D84">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1570,13 +1570,13 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>728.9613759228999</v>
+        <v>193.1700892535822</v>
       </c>
       <c r="C85">
-        <v>-0.6573187238851748</v>
+        <v>4.669553356224226</v>
       </c>
       <c r="D85">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1584,13 +1584,13 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>761.2963995621634</v>
+        <v>199.2378447907259</v>
       </c>
       <c r="C86">
-        <v>4.435766380396461</v>
+        <v>3.14114652045236</v>
       </c>
       <c r="D86">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1598,13 +1598,13 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>762.2319582822192</v>
+        <v>201.1236931250922</v>
       </c>
       <c r="C87">
-        <v>0.1228902068358479</v>
+        <v>0.9465311855522117</v>
       </c>
       <c r="D87">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1612,13 +1612,13 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>767.577432626388</v>
+        <v>202.3218684389207</v>
       </c>
       <c r="C88">
-        <v>0.7012923410106587</v>
+        <v>0.5957405093408086</v>
       </c>
       <c r="D88">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1626,13 +1626,13 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>784.2220273967741</v>
+        <v>203.9505709988495</v>
       </c>
       <c r="C89">
-        <v>2.16845806858</v>
+        <v>0.8050056934011333</v>
       </c>
       <c r="D89">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1640,13 +1640,13 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>806.1042936565144</v>
+        <v>200.2317318888091</v>
       </c>
       <c r="C90">
-        <v>2.790315178008773</v>
+        <v>-1.823402156624214</v>
       </c>
       <c r="D90">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1654,13 +1654,13 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>817.4866373408665</v>
+        <v>186.9094750545412</v>
       </c>
       <c r="C91">
-        <v>1.412018739252887</v>
+        <v>-6.653419369945738</v>
       </c>
       <c r="D91">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1668,13 +1668,13 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>815.9780487916818</v>
+        <v>184.5563238227425</v>
       </c>
       <c r="C92">
-        <v>-0.1845398420323951</v>
+        <v>-1.258979102644231</v>
       </c>
       <c r="D92">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1682,13 +1682,13 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>794.0485519524923</v>
+        <v>189.3691623611887</v>
       </c>
       <c r="C93">
-        <v>-2.687510634834249</v>
+        <v>2.607788472785479</v>
       </c>
       <c r="D93">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1696,13 +1696,13 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>807.3298739072225</v>
+        <v>187.1800761379913</v>
       </c>
       <c r="C94">
-        <v>1.672608296063581</v>
+        <v>-1.155988755456459</v>
       </c>
       <c r="D94">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1710,13 +1710,13 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>819.8036841537606</v>
+        <v>180.5933899409251</v>
       </c>
       <c r="C95">
-        <v>1.545069822099955</v>
+        <v>-3.518903471441283</v>
       </c>
       <c r="D95">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1724,13 +1724,13 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>818.1447356999787</v>
+        <v>183.4621461394472</v>
       </c>
       <c r="C96">
-        <v>-0.2023592337834377</v>
+        <v>1.588516722267952</v>
       </c>
       <c r="D96">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1738,13 +1738,13 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>799.3139714290819</v>
+        <v>195.2746749378565</v>
       </c>
       <c r="C97">
-        <v>-2.301642172736809</v>
+        <v>6.438673615771783</v>
       </c>
       <c r="D97">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1752,13 +1752,13 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>812.9659568311168</v>
+        <v>197.6477243197925</v>
       </c>
       <c r="C98">
-        <v>1.707962814365262</v>
+        <v>1.215236631524926</v>
       </c>
       <c r="D98">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1766,13 +1766,13 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>829.8623449876394</v>
+        <v>187.7272746777739</v>
       </c>
       <c r="C99">
-        <v>2.078363554408038</v>
+        <v>-5.019258216182339</v>
       </c>
       <c r="D99">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1780,13 +1780,13 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>803.4165138157098</v>
+        <v>180.2397504827084</v>
       </c>
       <c r="C100">
-        <v>-3.186773243979823</v>
+        <v>-3.988511636317936</v>
       </c>
       <c r="D100">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1794,13 +1794,13 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>785.320480002772</v>
+        <v>180.2993233093213</v>
       </c>
       <c r="C101">
-        <v>-2.252385095620368</v>
+        <v>0.03305199128014492</v>
       </c>
       <c r="D101">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1808,13 +1808,13 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>764.5612047683978</v>
+        <v>187.3445854707365</v>
       </c>
       <c r="C102">
-        <v>-2.643414473833774</v>
+        <v>3.907536662979255</v>
       </c>
       <c r="D102">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1822,13 +1822,13 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>754.5088703796673</v>
+        <v>190.7985809401522</v>
       </c>
       <c r="C103">
-        <v>-1.314784784532133</v>
+        <v>1.843659084535047</v>
       </c>
       <c r="D103">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1836,13 +1836,13 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>747.691353392087</v>
+        <v>199.4131900781827</v>
       </c>
       <c r="C104">
-        <v>-0.9035701573859205</v>
+        <v>4.51502788730519</v>
       </c>
       <c r="D104">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1850,13 +1850,13 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>765.540881038714</v>
+        <v>206.9517884369828</v>
       </c>
       <c r="C105">
-        <v>2.387285551136609</v>
+        <v>3.780391034236274</v>
       </c>
       <c r="D105">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1864,13 +1864,13 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>780.759715318924</v>
+        <v>207.9428184288703</v>
       </c>
       <c r="C106">
-        <v>1.987984529259957</v>
+        <v>0.4788699819277832</v>
       </c>
       <c r="D106">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1878,13 +1878,13 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>769.2292921815265</v>
+        <v>191.2203063642841</v>
       </c>
       <c r="C107">
-        <v>-1.476820961835557</v>
+        <v>-8.041880066325193</v>
       </c>
       <c r="D107">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1892,13 +1892,13 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>767.9349256236519</v>
+        <v>196.57302538913</v>
       </c>
       <c r="C108">
-        <v>-0.1682679756258011</v>
+        <v>2.799241945909556</v>
       </c>
       <c r="D108">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1906,13 +1906,13 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>800.9368908986869</v>
+        <v>202.0625864615587</v>
       </c>
       <c r="C109">
-        <v>4.297495031656965</v>
+        <v>2.792631929819368</v>
       </c>
       <c r="D109">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1920,13 +1920,13 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>799.9846649514761</v>
+        <v>202.0666179748651</v>
       </c>
       <c r="C110">
-        <v>-0.1188890108610532</v>
+        <v>0.001995180491808246</v>
       </c>
       <c r="D110">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1934,13 +1934,13 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>830.4152894272262</v>
+        <v>199.1351879279287</v>
       </c>
       <c r="C111">
-        <v>3.803900975726311</v>
+        <v>-1.450724556245621</v>
       </c>
       <c r="D111">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1948,13 +1948,13 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>861.4157642032022</v>
+        <v>208.6805054193597</v>
       </c>
       <c r="C112">
-        <v>3.733129094643526</v>
+        <v>4.793385634529678</v>
       </c>
       <c r="D112">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -1962,13 +1962,13 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>872.6991230834269</v>
+        <v>199.2421417784343</v>
       </c>
       <c r="C113">
-        <v>1.30986213035719</v>
+        <v>-4.5228775069134</v>
       </c>
       <c r="D113">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -1976,13 +1976,13 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>855.4019292441831</v>
+        <v>195.9953085345008</v>
       </c>
       <c r="C114">
-        <v>-1.982034057525947</v>
+        <v>-1.629591618997984</v>
       </c>
       <c r="D114">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -1990,13 +1990,13 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>865.6642169436276</v>
+        <v>195.5720010550067</v>
       </c>
       <c r="C115">
-        <v>1.199703595304273</v>
+        <v>-0.2159783734923406</v>
       </c>
       <c r="D115">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2004,13 +2004,13 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>857.4117970441132</v>
+        <v>191.7694303090576</v>
       </c>
       <c r="C116">
-        <v>-0.9533049579721556</v>
+        <v>-1.944332892968456</v>
       </c>
       <c r="D116">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2018,13 +2018,13 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>875.8473179634318</v>
+        <v>197.434706097931</v>
       </c>
       <c r="C117">
-        <v>2.1501361402857</v>
+        <v>2.954212138891595</v>
       </c>
       <c r="D117">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2032,13 +2032,13 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>896.4200923118069</v>
+        <v>205.2548606512526</v>
       </c>
       <c r="C118">
-        <v>2.348899622848879</v>
+        <v>3.960881401187208</v>
       </c>
       <c r="D118">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2046,13 +2046,13 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>916.809803420873</v>
+        <v>195.3857097273716</v>
       </c>
       <c r="C119">
-        <v>2.274570961086161</v>
+        <v>-4.808242247012925</v>
       </c>
       <c r="D119">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2060,13 +2060,13 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>898.5918942666203</v>
+        <v>185.0157534864875</v>
       </c>
       <c r="C120">
-        <v>-1.987097987638934</v>
+        <v>-5.307428191833295</v>
       </c>
       <c r="D120">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2074,13 +2074,13 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>882.1400580676907</v>
+        <v>174.2229950115272</v>
       </c>
       <c r="C121">
-        <v>-1.830846272250958</v>
+        <v>-5.833426760466939</v>
       </c>
       <c r="D121">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2088,13 +2088,13 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>844.9844610084057</v>
+        <v>177.9966654482122</v>
       </c>
       <c r="C122">
-        <v>-4.211983881638198</v>
+        <v>2.166000209349722</v>
       </c>
       <c r="D122">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2102,13 +2102,13 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>806.8004315071597</v>
+        <v>183.2357277423576</v>
       </c>
       <c r="C123">
-        <v>-4.518903158961897</v>
+        <v>2.943348562712051</v>
       </c>
       <c r="D123">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2116,13 +2116,13 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>852.5163560037225</v>
+        <v>187.4656171445446</v>
       </c>
       <c r="C124">
-        <v>5.666323753838634</v>
+        <v>2.308441401850711</v>
       </c>
       <c r="D124">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2130,13 +2130,13 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>820.1474633193247</v>
+        <v>195.4109538463532</v>
       </c>
       <c r="C125">
-        <v>-3.796864711913693</v>
+        <v>4.238290105050248</v>
       </c>
       <c r="D125">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2144,13 +2144,13 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>800.5058271251943</v>
+        <v>198.6760294462464</v>
       </c>
       <c r="C126">
-        <v>-2.394890805933393</v>
+        <v>1.670876445575538</v>
       </c>
       <c r="D126">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2158,13 +2158,13 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>754.8208332765453</v>
+        <v>204.3563727453357</v>
       </c>
       <c r="C127">
-        <v>-5.707015776851327</v>
+        <v>2.859098460403897</v>
       </c>
       <c r="D127">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2172,13 +2172,13 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>734.7723026717637</v>
+        <v>210.1790123253483</v>
       </c>
       <c r="C128">
-        <v>-2.656064819747278</v>
+        <v>2.849257648191213</v>
       </c>
       <c r="D128">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2186,13 +2186,13 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>716.6441800273119</v>
+        <v>216.8640383223829</v>
       </c>
       <c r="C129">
-        <v>-2.467175556091964</v>
+        <v>3.180634414004414</v>
       </c>
       <c r="D129">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2200,13 +2200,13 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>738.4315650229362</v>
+        <v>222.6290099451202</v>
       </c>
       <c r="C130">
-        <v>3.040195623272059</v>
+        <v>2.658334534085958</v>
       </c>
       <c r="D130">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2214,13 +2214,13 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>728.0896539528691</v>
+        <v>218.0463729513223</v>
       </c>
       <c r="C131">
-        <v>-1.40052396998304</v>
+        <v>-2.058418619805025</v>
       </c>
       <c r="D131">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2228,13 +2228,13 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>709.480982250343</v>
+        <v>207.5902659667381</v>
       </c>
       <c r="C132">
-        <v>-2.555821470817194</v>
+        <v>-4.795359282091111</v>
       </c>
       <c r="D132">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2242,13 +2242,13 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>684.7785921903227</v>
+        <v>201.8455237251258</v>
       </c>
       <c r="C133">
-        <v>-3.481755068567016</v>
+        <v>-2.767346635864271</v>
       </c>
       <c r="D133">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2256,13 +2256,13 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>682.6574614715865</v>
+        <v>196.7235541396055</v>
       </c>
       <c r="C134">
-        <v>-0.3097542392427166</v>
+        <v>-2.537569073117258</v>
       </c>
       <c r="D134">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2270,13 +2270,13 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>663.8797000785727</v>
+        <v>197.1158240014498</v>
       </c>
       <c r="C135">
-        <v>-2.750685732275626</v>
+        <v>0.1994015732177635</v>
       </c>
       <c r="D135">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2284,13 +2284,13 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>664.1140574925739</v>
+        <v>186.8838158329986</v>
       </c>
       <c r="C136">
-        <v>0.03530118694298222</v>
+        <v>-5.19086086583078</v>
       </c>
       <c r="D136">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2298,13 +2298,13 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>668.569622300642</v>
+        <v>186.345200016284</v>
       </c>
       <c r="C137">
-        <v>0.6709035530569049</v>
+        <v>-0.2882089143534583</v>
       </c>
       <c r="D137">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2312,13 +2312,13 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>701.2923462562517</v>
+        <v>179.86300019776</v>
       </c>
       <c r="C138">
-        <v>4.894437746514139</v>
+        <v>-3.478597687494806</v>
       </c>
       <c r="D138">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2326,13 +2326,13 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>678.1639931330021</v>
+        <v>183.3038188888874</v>
       </c>
       <c r="C139">
-        <v>-3.297961719775913</v>
+        <v>1.913021959682759</v>
       </c>
       <c r="D139">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2340,13 +2340,13 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>673.8465616091755</v>
+        <v>186.511733120185</v>
       </c>
       <c r="C140">
-        <v>-0.6366353223621851</v>
+        <v>1.750053136231787</v>
       </c>
       <c r="D140">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2354,13 +2354,13 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>653.7789428606291</v>
+        <v>190.3412447724293</v>
       </c>
       <c r="C141">
-        <v>-2.978069473356678</v>
+        <v>2.05322828123455</v>
       </c>
       <c r="D141">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2368,13 +2368,13 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>702.6143884539896</v>
+        <v>190.2246151592614</v>
       </c>
       <c r="C142">
-        <v>7.469718339302821</v>
+        <v>-0.06127395736398018</v>
       </c>
       <c r="D142">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2382,13 +2382,13 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>709.9013852728795</v>
+        <v>189.1886605126023</v>
       </c>
       <c r="C143">
-        <v>1.037126045044988</v>
+        <v>-0.5445954750870788</v>
       </c>
       <c r="D143">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2396,13 +2396,13 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>703.63063646365</v>
+        <v>183.6642964378292</v>
       </c>
       <c r="C144">
-        <v>-0.8833267464070323</v>
+        <v>-2.920029170778498</v>
       </c>
       <c r="D144">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2410,13 +2410,13 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>680.3020859380686</v>
+        <v>179.0791616696036</v>
       </c>
       <c r="C145">
-        <v>-3.31545406306177</v>
+        <v>-2.496475829627358</v>
       </c>
       <c r="D145">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2424,13 +2424,13 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>642.9451304431668</v>
+        <v>177.3142955147091</v>
       </c>
       <c r="C146">
-        <v>-5.491230479381858</v>
+        <v>-0.985522904195123</v>
       </c>
       <c r="D146">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2438,13 +2438,13 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>642.1241597124711</v>
+        <v>178.4043897693539</v>
       </c>
       <c r="C147">
-        <v>-0.127689081357508</v>
+        <v>0.6147808057328005</v>
       </c>
       <c r="D147">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2452,13 +2452,13 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>645.0157744414919</v>
+        <v>179.6482355805842</v>
       </c>
       <c r="C148">
-        <v>0.4503201889048481</v>
+        <v>0.6972058326807229</v>
       </c>
       <c r="D148">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2466,13 +2466,13 @@
         <v>147</v>
       </c>
       <c r="B149">
-        <v>637.8722232892069</v>
+        <v>168.9772051914959</v>
       </c>
       <c r="C149">
-        <v>-1.107500224854259</v>
+        <v>-5.939958360627301</v>
       </c>
       <c r="D149">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2480,13 +2480,13 @@
         <v>148</v>
       </c>
       <c r="B150">
-        <v>676.491126076557</v>
+        <v>168.6871879658811</v>
       </c>
       <c r="C150">
-        <v>6.054332102471956</v>
+        <v>-0.1716309754834184</v>
       </c>
       <c r="D150">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2494,13 +2494,13 @@
         <v>149</v>
       </c>
       <c r="B151">
-        <v>655.0028613648411</v>
+        <v>160.8023713072446</v>
       </c>
       <c r="C151">
-        <v>-3.176429650502777</v>
+        <v>-4.674223782917836</v>
       </c>
       <c r="D151">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2508,13 +2508,13 @@
         <v>150</v>
       </c>
       <c r="B152">
-        <v>678.3890991046145</v>
+        <v>165.1210683931321</v>
       </c>
       <c r="C152">
-        <v>3.570402378249625</v>
+        <v>2.685717288108779</v>
       </c>
       <c r="D152">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2522,13 +2522,13 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>674.8232203465159</v>
+        <v>175.6973009351858</v>
       </c>
       <c r="C153">
-        <v>-0.5256391594153091</v>
+        <v>6.405138148012114</v>
       </c>
       <c r="D153">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2536,13 +2536,13 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>659.118162662406</v>
+        <v>177.9554883545442</v>
       </c>
       <c r="C154">
-        <v>-2.327284718514207</v>
+        <v>1.285271547905789</v>
       </c>
       <c r="D154">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2550,13 +2550,13 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>660.5029979370336</v>
+        <v>181.6550096244775</v>
       </c>
       <c r="C155">
-        <v>0.2101042503568297</v>
+        <v>2.078902597576906</v>
       </c>
       <c r="D155">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2564,13 +2564,13 @@
         <v>154</v>
       </c>
       <c r="B156">
-        <v>634.8806362057071</v>
+        <v>189.1525649129771</v>
       </c>
       <c r="C156">
-        <v>-3.87921959648229</v>
+        <v>4.127359495341657</v>
       </c>
       <c r="D156">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2578,13 +2578,13 @@
         <v>155</v>
       </c>
       <c r="B157">
-        <v>611.7800213988859</v>
+        <v>199.9719671556883</v>
       </c>
       <c r="C157">
-        <v>-3.638576055001377</v>
+        <v>5.719934195811095</v>
       </c>
       <c r="D157">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2592,13 +2592,13 @@
         <v>156</v>
       </c>
       <c r="B158">
-        <v>621.2751695659441</v>
+        <v>207.8722414921369</v>
       </c>
       <c r="C158">
-        <v>1.552052671701625</v>
+        <v>3.950690913740859</v>
       </c>
       <c r="D158">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2606,13 +2606,13 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>646.1505784510819</v>
+        <v>204.624636527105</v>
       </c>
       <c r="C159">
-        <v>4.003927744692754</v>
+        <v>-1.562308147408314</v>
       </c>
       <c r="D159">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2620,13 +2620,13 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>644.2523318436048</v>
+        <v>196.3373643238011</v>
       </c>
       <c r="C160">
-        <v>-0.2937777463617642</v>
+        <v>-4.049987500994846</v>
       </c>
       <c r="D160">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2634,13 +2634,13 @@
         <v>159</v>
       </c>
       <c r="B161">
-        <v>652.35411224825</v>
+        <v>197.6644904475475</v>
       </c>
       <c r="C161">
-        <v>1.257547703624289</v>
+        <v>0.6759417028526847</v>
       </c>
       <c r="D161">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -2648,13 +2648,13 @@
         <v>160</v>
       </c>
       <c r="B162">
-        <v>635.3555006831645</v>
+        <v>199.6080558619848</v>
       </c>
       <c r="C162">
-        <v>-2.60573379487133</v>
+        <v>0.9832648292249097</v>
       </c>
       <c r="D162">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -2662,13 +2662,13 @@
         <v>161</v>
       </c>
       <c r="B163">
-        <v>652.6164236809562</v>
+        <v>192.6824340304709</v>
       </c>
       <c r="C163">
-        <v>2.71673464371239</v>
+        <v>-3.469610383011046</v>
       </c>
       <c r="D163">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2676,13 +2676,13 @@
         <v>162</v>
       </c>
       <c r="B164">
-        <v>648.2278537143595</v>
+        <v>188.1881495473975</v>
       </c>
       <c r="C164">
-        <v>-0.6724577879673718</v>
+        <v>-2.332482722510491</v>
       </c>
       <c r="D164">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -2690,13 +2690,13 @@
         <v>163</v>
       </c>
       <c r="B165">
-        <v>648.9114740263046</v>
+        <v>194.308941097324</v>
       </c>
       <c r="C165">
-        <v>0.1054598792736063</v>
+        <v>3.252485113779659</v>
       </c>
       <c r="D165">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -2704,13 +2704,13 @@
         <v>164</v>
       </c>
       <c r="B166">
-        <v>656.2184744789657</v>
+        <v>184.0892507731066</v>
       </c>
       <c r="C166">
-        <v>1.126039644101729</v>
+        <v>-5.259505952996073</v>
       </c>
       <c r="D166">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2718,13 +2718,13 @@
         <v>165</v>
       </c>
       <c r="B167">
-        <v>655.4777944080364</v>
+        <v>185.6559941385798</v>
       </c>
       <c r="C167">
-        <v>-0.1128709568131917</v>
+        <v>0.8510781367697463</v>
       </c>
       <c r="D167">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -2732,13 +2732,13 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>670.8548291193412</v>
+        <v>184.273146755968</v>
       </c>
       <c r="C168">
-        <v>2.345927633626668</v>
+        <v>-0.7448439190062331</v>
       </c>
       <c r="D168">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2746,13 +2746,13 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>659.5790718806367</v>
+        <v>173.8346419962909</v>
       </c>
       <c r="C169">
-        <v>-1.680804363219192</v>
+        <v>-5.664691217055501</v>
       </c>
       <c r="D169">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2760,13 +2760,13 @@
         <v>168</v>
       </c>
       <c r="B170">
-        <v>664.8792417321969</v>
+        <v>169.5659319791349</v>
       </c>
       <c r="C170">
-        <v>0.8035685299183246</v>
+        <v>-2.4556152721545</v>
       </c>
       <c r="D170">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2774,13 +2774,13 @@
         <v>169</v>
       </c>
       <c r="B171">
-        <v>664.2186163296868</v>
+        <v>166.1973561703783</v>
       </c>
       <c r="C171">
-        <v>-0.09936020874843016</v>
+        <v>-1.986587617830591</v>
       </c>
       <c r="D171">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -2788,13 +2788,13 @@
         <v>170</v>
       </c>
       <c r="B172">
-        <v>660.7459862587582</v>
+        <v>165.5946227773117</v>
       </c>
       <c r="C172">
-        <v>-0.5228143243135109</v>
+        <v>-0.3626612401997429</v>
       </c>
       <c r="D172">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2802,13 +2802,13 @@
         <v>171</v>
       </c>
       <c r="B173">
-        <v>686.697080945069</v>
+        <v>165.9305113651719</v>
       </c>
       <c r="C173">
-        <v>3.927544809352495</v>
+        <v>0.2028378592413231</v>
       </c>
       <c r="D173">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -2816,13 +2816,13 @@
         <v>172</v>
       </c>
       <c r="B174">
-        <v>667.3714966588177</v>
+        <v>170.7310415136207</v>
       </c>
       <c r="C174">
-        <v>-2.814280826657143</v>
+        <v>2.89309669990951</v>
       </c>
       <c r="D174">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -2830,13 +2830,13 @@
         <v>173</v>
       </c>
       <c r="B175">
-        <v>720.7048760802354</v>
+        <v>171.2927796956717</v>
       </c>
       <c r="C175">
-        <v>7.991557878697275</v>
+        <v>0.3290193611372054</v>
       </c>
       <c r="D175">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -2844,13 +2844,13 @@
         <v>174</v>
       </c>
       <c r="B176">
-        <v>724.1504165408379</v>
+        <v>169.5768997144441</v>
       </c>
       <c r="C176">
-        <v>0.478079249212534</v>
+        <v>-1.001723472685809</v>
       </c>
       <c r="D176">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -2858,13 +2858,13 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>714.3135407655851</v>
+        <v>171.6735553029569</v>
       </c>
       <c r="C177">
-        <v>-1.358402280874479</v>
+        <v>1.236404010241629</v>
       </c>
       <c r="D177">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -2872,13 +2872,13 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>691.0567295941324</v>
+        <v>164.3143717987757</v>
       </c>
       <c r="C178">
-        <v>-3.255826726527767</v>
+        <v>-4.286730994295694</v>
       </c>
       <c r="D178">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -2886,13 +2886,13 @@
         <v>177</v>
       </c>
       <c r="B179">
-        <v>697.6754075445198</v>
+        <v>162.8479807502197</v>
       </c>
       <c r="C179">
-        <v>0.9577618836408156</v>
+        <v>-0.8924301827668795</v>
       </c>
       <c r="D179">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -2900,13 +2900,13 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>734.245462913841</v>
+        <v>158.5512363547356</v>
       </c>
       <c r="C180">
-        <v>5.241700506261233</v>
+        <v>-2.638500259990679</v>
       </c>
       <c r="D180">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -2914,13 +2914,13 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>705.6618277311239</v>
+        <v>162.3681376157578</v>
       </c>
       <c r="C181">
-        <v>-3.892926361340174</v>
+        <v>2.407361398609642</v>
       </c>
       <c r="D181">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -2928,13 +2928,13 @@
         <v>180</v>
       </c>
       <c r="B182">
-        <v>710.6416820654994</v>
+        <v>161.9902043591663</v>
       </c>
       <c r="C182">
-        <v>0.7056998322251489</v>
+        <v>-0.2327631899590604</v>
       </c>
       <c r="D182">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -2942,13 +2942,13 @@
         <v>181</v>
       </c>
       <c r="B183">
-        <v>702.507330548498</v>
+        <v>164.4539398873723</v>
       </c>
       <c r="C183">
-        <v>-1.144648804353642</v>
+        <v>1.520916365253424</v>
       </c>
       <c r="D183">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -2956,13 +2956,13 @@
         <v>182</v>
       </c>
       <c r="B184">
-        <v>689.7583731562041</v>
+        <v>166.2857552103762</v>
       </c>
       <c r="C184">
-        <v>-1.814779268187827</v>
+        <v>1.113877432342704</v>
       </c>
       <c r="D184">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -2970,13 +2970,13 @@
         <v>183</v>
       </c>
       <c r="B185">
-        <v>660.313008877928</v>
+        <v>165.3958527186218</v>
       </c>
       <c r="C185">
-        <v>-4.268939011720817</v>
+        <v>-0.535164597008629</v>
       </c>
       <c r="D185">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -2984,13 +2984,13 @@
         <v>184</v>
       </c>
       <c r="B186">
-        <v>643.5435352654908</v>
+        <v>161.4003104642056</v>
       </c>
       <c r="C186">
-        <v>-2.539624903185483</v>
+        <v>-2.415745128273323</v>
       </c>
       <c r="D186">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -2998,13 +2998,13 @@
         <v>185</v>
       </c>
       <c r="B187">
-        <v>652.1253216176763</v>
+        <v>158.2839721833965</v>
       </c>
       <c r="C187">
-        <v>1.333520714903158</v>
+        <v>-1.930813064637939</v>
       </c>
       <c r="D187">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3012,13 +3012,13 @@
         <v>186</v>
       </c>
       <c r="B188">
-        <v>674.661187977893</v>
+        <v>158.012606363011</v>
       </c>
       <c r="C188">
-        <v>3.455756986143966</v>
+        <v>-0.1714423871489998</v>
       </c>
       <c r="D188">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3026,13 +3026,13 @@
         <v>187</v>
       </c>
       <c r="B189">
-        <v>667.2523745358096</v>
+        <v>159.3107810421007</v>
       </c>
       <c r="C189">
-        <v>-1.098153202541443</v>
+        <v>0.8215639935128649</v>
       </c>
       <c r="D189">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3040,13 +3040,13 @@
         <v>188</v>
       </c>
       <c r="B190">
-        <v>698.933746204152</v>
+        <v>156.7709677071408</v>
       </c>
       <c r="C190">
-        <v>4.748034308665045</v>
+        <v>-1.594250758389491</v>
       </c>
       <c r="D190">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3054,13 +3054,13 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>701.3346939208715</v>
+        <v>162.0016320370079</v>
       </c>
       <c r="C191">
-        <v>0.3435157809676264</v>
+        <v>3.33650063297326</v>
       </c>
       <c r="D191">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3068,13 +3068,13 @@
         <v>190</v>
       </c>
       <c r="B192">
-        <v>684.9899828982858</v>
+        <v>163.9223322059936</v>
       </c>
       <c r="C192">
-        <v>-2.33051511129574</v>
+        <v>1.185605444114888</v>
       </c>
       <c r="D192">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -3082,13 +3082,13 @@
         <v>191</v>
       </c>
       <c r="B193">
-        <v>672.9156134520292</v>
+        <v>170.8817107937284</v>
       </c>
       <c r="C193">
-        <v>-1.762707447949567</v>
+        <v>4.245534146615999</v>
       </c>
       <c r="D193">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3096,13 +3096,13 @@
         <v>192</v>
       </c>
       <c r="B194">
-        <v>679.0081805326026</v>
+        <v>173.3435663782781</v>
       </c>
       <c r="C194">
-        <v>0.9053983826172155</v>
+        <v>1.440678217179934</v>
       </c>
       <c r="D194">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3110,13 +3110,13 @@
         <v>193</v>
       </c>
       <c r="B195">
-        <v>689.708263329264</v>
+        <v>162.3070183905685</v>
       </c>
       <c r="C195">
-        <v>1.575840041907657</v>
+        <v>-6.366863344454956</v>
       </c>
       <c r="D195">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3124,13 +3124,13 @@
         <v>194</v>
       </c>
       <c r="B196">
-        <v>684.8753014167811</v>
+        <v>169.8459744144373</v>
       </c>
       <c r="C196">
-        <v>-0.7007255341778735</v>
+        <v>4.644873708250445</v>
       </c>
       <c r="D196">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3138,13 +3138,13 @@
         <v>195</v>
       </c>
       <c r="B197">
-        <v>690.2317372856613</v>
+        <v>164.0002620332838</v>
       </c>
       <c r="C197">
-        <v>0.7821038162420948</v>
+        <v>-3.441772701005829</v>
       </c>
       <c r="D197">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3152,13 +3152,13 @@
         <v>196</v>
       </c>
       <c r="B198">
-        <v>707.4998021517471</v>
+        <v>166.1647052869197</v>
       </c>
       <c r="C198">
-        <v>2.501777871587376</v>
+        <v>1.319780363031736</v>
       </c>
       <c r="D198">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3166,13 +3166,13 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>704.3600190706013</v>
+        <v>166.9006577178895</v>
       </c>
       <c r="C199">
-        <v>-0.4437857186103333</v>
+        <v>0.442905386976737</v>
       </c>
       <c r="D199">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3180,13 +3180,13 @@
         <v>198</v>
       </c>
       <c r="B200">
-        <v>718.6647227089582</v>
+        <v>167.2798780775638</v>
       </c>
       <c r="C200">
-        <v>2.030879557478547</v>
+        <v>0.2272132206424833</v>
       </c>
       <c r="D200">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3194,13 +3194,13 @@
         <v>199</v>
       </c>
       <c r="B201">
-        <v>735.9888881257639</v>
+        <v>166.1307630741817</v>
       </c>
       <c r="C201">
-        <v>2.410604676893488</v>
+        <v>-0.6869415596114135</v>
       </c>
       <c r="D201">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>